<commit_message>
BIG CHANGE: COMPLETE UPDATE RULE SET, resolve odd numbered players in rule set being ommitted
</commit_message>
<xml_diff>
--- a/Player ages and rule set.xlsx
+++ b/Player ages and rule set.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rossritchie/code/fantasy_trade_calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7137C6-A4B2-E94A-B3F7-6F73F5D12014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E31ED1-12F5-3E4D-B83A-DE0114E35635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30820" yWindow="2760" windowWidth="35960" windowHeight="17860" activeTab="1" xr2:uid="{ADC212AB-1DA1-2647-8168-12F8CA61FD89}"/>
+    <workbookView xWindow="2240" yWindow="500" windowWidth="26100" windowHeight="16000" activeTab="1" xr2:uid="{ADC212AB-1DA1-2647-8168-12F8CA61FD89}"/>
   </bookViews>
   <sheets>
     <sheet name="Player ages" sheetId="1" r:id="rId1"/>
     <sheet name="Rule set" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -4403,7 +4403,7 @@
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>